<commit_message>
update deploy 2105. add enrypted vtl
</commit_message>
<xml_diff>
--- a/AAA/myRepo-master/cypress/fixtures/mobi2.xlsx
+++ b/AAA/myRepo-master/cypress/fixtures/mobi2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -367,7 +367,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>